<commit_message>
Update Nov 6, 2025
Updated Arcaea 6.10.5
Removed Arcaea 6.8.2_2, 6.8.2_3 since both have the same SHA-256
Updated 植物大战僵尸2 3.8.8_1725
</commit_message>
<xml_diff>
--- a/arcaea.xlsx
+++ b/arcaea.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myth1\OneDrive\Desktop\Project\Project-apk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D12CCD0-36F5-443F-A253-19B65DB41CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE7DBC1-F16F-481D-A9E4-01582C8D5D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="87">
   <si>
     <t>Version</t>
   </si>
@@ -68,12 +68,6 @@
     <t>Oct 14, 2025</t>
   </si>
   <si>
-    <t>6.9.4</t>
-  </si>
-  <si>
-    <t>6.9.2</t>
-  </si>
-  <si>
     <t>Unknown</t>
   </si>
   <si>
@@ -131,24 +125,6 @@
     <t>6.7.0</t>
   </si>
   <si>
-    <t>6.8.2_3</t>
-  </si>
-  <si>
-    <t>6.8.2_2</t>
-  </si>
-  <si>
-    <t>6.8.2_1</t>
-  </si>
-  <si>
-    <t>https://pan.baidu.com/s/1a-Z7xRaIL_jQXl1yXrO6xw?pwd=1234</t>
-  </si>
-  <si>
-    <t>https://pan.baidu.com/s/1hEust2y9lRSqzytwj2DnGw?pwd=1234</t>
-  </si>
-  <si>
-    <t>https://pan.baidu.com/s/14dBO3m9WRid0u4GNHwbu2A?pwd=1234</t>
-  </si>
-  <si>
     <t>https://pan.baidu.com/s/1CQhZJXfyP2oBNGuMrXNpQw?pwd=1234</t>
   </si>
   <si>
@@ -161,12 +137,6 @@
     <t>https://pan.baidu.com/s/1bWmVjNHcJtQ_7Jum9RiulA?pwd=1234</t>
   </si>
   <si>
-    <t>https://arcaea-static.lowiro-cdn.net/QyzLJrrUpstku0EwifX7genroAiFOz8rMBSjjwmIOPhsV7djwrv%2BHt%2BYkd07uEF3L1VoSEmVFz1TpD%2B7xJrPqWNJ5BoNKJihzNOVZYrxwGkTEgkEEm4v1Ieh6%2BAEBvJIPtWDgZrpI28tRaY%3D?filename=arcaea_6.8.2c.apk</t>
-  </si>
-  <si>
-    <t>https://arcaea-static.lowiro-cdn.net/JpT4PPAiB2Sh99ALcjkoWqs%2Fu4OL6dqpj%2FQKONKyqhlF2OUnxfssztkQn0fYQuAdjjEtv5fsfzKMxn0M0KSUpGnb5Wt6E%2FtRQPedCr5k4sERSrjGzW20F%2BW8G%2FhuM82HwiGCfvm0fDTkesM%3D?filename=arcaea_6.8.2c.apk</t>
-  </si>
-  <si>
     <t>https://arcaea-static.lowiro-cdn.net/X8zlPRgN0CRl1N7vNUf4dhiTgzuseZyQkcm0a%2F5fLfN4G3VUCuK%2F9KGrNpkUqEtdd2i9zAUt%2Fg1J5fznKYltAgD3VGP02JDuJ80CT%2BU5ZRUp1SqQO6tmKywi%2F4MMK%2F18YGzSXUuO2JEN9sU%3D?filename=arcaea_6.8.2c.apk</t>
   </si>
   <si>
@@ -194,12 +164,6 @@
     <t>https://pan.baidu.com/s/1ZJBdI1R5XIy1MGc6G_DG3Q?pwd=1234</t>
   </si>
   <si>
-    <t>Sep 7. 2025</t>
-  </si>
-  <si>
-    <t>Sep 6, 2025</t>
-  </si>
-  <si>
     <t>Sep 3, 2025</t>
   </si>
   <si>
@@ -218,9 +182,6 @@
     <t>Jun 26, 2025</t>
   </si>
   <si>
-    <t>6.9.6</t>
-  </si>
-  <si>
     <t>Oct 25, 2025</t>
   </si>
   <si>
@@ -272,9 +233,6 @@
     <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.8.1c.apk</t>
   </si>
   <si>
-    <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.8.2c_1.apk</t>
-  </si>
-  <si>
     <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.9.1c.apk</t>
   </si>
   <si>
@@ -287,12 +245,6 @@
     <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.8.4c.apk</t>
   </si>
   <si>
-    <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.8.2c_3.apk</t>
-  </si>
-  <si>
-    <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.8.2c_2.apk</t>
-  </si>
-  <si>
     <t>6.10.1</t>
   </si>
   <si>
@@ -318,6 +270,30 @@
   </si>
   <si>
     <t>Nov 2, 2025</t>
+  </si>
+  <si>
+    <t>6.10.5</t>
+  </si>
+  <si>
+    <t>Nov 6, 2025</t>
+  </si>
+  <si>
+    <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.10.5c.apk</t>
+  </si>
+  <si>
+    <t>https://arcaea-static.lowiro-cdn.net/JMRuNFwy%2FSj6vyJ5tim%2BJepa0Isz4wBA3D7uhkoHHZtVI5rx1cV9E39jjTPUFATLPm0%2FDqMuc4huxIQ6gvawS5AdDJjYzwjMBm5CKFmurFkJJchbZ172Aj%2FP9CY1eG%2BtTYqzyP4Xh1MWvuztMw%3D%3D?filename=arcaea_6.10.5c.apk</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1TOJxBl9xEGBxNxMDNFtAUg?pwd=1234</t>
+  </si>
+  <si>
+    <t>https://pan.baidu.com/s/1-pKjmy5M8Y1umPa3uCmMoA?pwd=1234</t>
+  </si>
+  <si>
+    <t>6.8.2</t>
+  </si>
+  <si>
+    <t>https://github.com/A-Randomm-User/APK-save/releases/download/Arcaea/arcaea_6.8.2c.apk</t>
   </si>
 </sst>
 </file>
@@ -387,13 +363,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -729,11 +706,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88782FC7-6F7E-9E4F-AEC6-757ED4B54885}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -754,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -765,87 +742,87 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>71</v>
+        <v>53</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -856,275 +833,209 @@
         <v>10</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>82</v>
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>27</v>
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{1D60641F-9F3C-4AF2-8E47-0C250005FA91}"/>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{1D60641F-9F3C-4AF2-8E47-0C250005FA91}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{DB78D329-2FDB-4E23-BC81-6801C720DF64}"/>
+    <hyperlink ref="E12" r:id="rId3" xr:uid="{645F2658-8B78-4D4A-95FA-F2FE2CE15078}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>